<commit_message>
test data -- there seems to be a problem with the date column. not sure this fixes it
</commit_message>
<xml_diff>
--- a/inst/extdata/test_file.xlsx
+++ b/inst/extdata/test_file.xlsx
@@ -129,13 +129,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="YYYY/MM/DD;@"/>
+    <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -258,10 +259,10 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8061224489796"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
@@ -273,7 +274,7 @@
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.8061224489796"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -305,7 +306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -337,7 +338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>